<commit_message>
added all some pictures and updated documents
</commit_message>
<xml_diff>
--- a/Thrust_Against_Mass_Calculations.xlsx
+++ b/Thrust_Against_Mass_Calculations.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="323" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Exp_data" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="PID_Values" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>M</t>
   </si>
@@ -42,6 +44,84 @@
   </si>
   <si>
     <t>T_hover/T_5</t>
+  </si>
+  <si>
+    <t>Length of pod</t>
+  </si>
+  <si>
+    <t>Perching time (minutes)</t>
+  </si>
+  <si>
+    <t>Hover time (seconds)</t>
+  </si>
+  <si>
+    <t>Oscillation amplitude (0 deg, aluminium plate)</t>
+  </si>
+  <si>
+    <t>Max angle (flat aluminium plate)</t>
+  </si>
+  <si>
+    <t>very difficult to keep stable</t>
+  </si>
+  <si>
+    <t>Should perform these tests at least two times\ each</t>
+  </si>
+  <si>
+    <t>Pod length (cm)</t>
+  </si>
+  <si>
+    <t>A_pkp</t>
+  </si>
+  <si>
+    <t>A_pki</t>
+  </si>
+  <si>
+    <t>A_pkd</t>
+  </si>
+  <si>
+    <t>A_rkp</t>
+  </si>
+  <si>
+    <t>A_rki</t>
+  </si>
+  <si>
+    <t>a_rkd</t>
+  </si>
+  <si>
+    <t>a_ykp</t>
+  </si>
+  <si>
+    <t>a_yki</t>
+  </si>
+  <si>
+    <t>a_ykd</t>
+  </si>
+  <si>
+    <t>r_pkp</t>
+  </si>
+  <si>
+    <t>r_pki</t>
+  </si>
+  <si>
+    <t>r_pkd</t>
+  </si>
+  <si>
+    <t>r_rkp</t>
+  </si>
+  <si>
+    <t>r_rki</t>
+  </si>
+  <si>
+    <t>r_rkd</t>
+  </si>
+  <si>
+    <t>r_ykp</t>
+  </si>
+  <si>
+    <t>r_yki</t>
+  </si>
+  <si>
+    <t>r_ykd</t>
   </si>
 </sst>
 </file>
@@ -56,6 +136,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,7 +220,7 @@
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K63" activeCellId="0" sqref="K63"/>
     </sheetView>
   </sheetViews>
@@ -1298,4 +1379,588 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>1050</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>2600</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>2600</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>2800</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>2800</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>3200</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>3200</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>5500</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>5500</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I have added the latest report version
</commit_message>
<xml_diff>
--- a/Thrust_Against_Mass_Calculations.xlsx
+++ b/Thrust_Against_Mass_Calculations.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>M</t>
   </si>
@@ -49,7 +49,10 @@
     <t>Length of pod</t>
   </si>
   <si>
-    <t>Perching time (minutes)</t>
+    <t>Perching time (minutes), trial    1</t>
+  </si>
+  <si>
+    <t>Perching time (minutes), trial    2</t>
   </si>
   <si>
     <t>Hover time (seconds)</t>
@@ -65,6 +68,15 @@
   </si>
   <si>
     <t>Should perform these tests at least two times each</t>
+  </si>
+  <si>
+    <t>No monopod</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>6 min 45 seconds (285 seconds)</t>
   </si>
   <si>
     <t>Pod length (cm)</t>
@@ -131,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -152,6 +164,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -278,10 +296,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>50</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -313,38 +351,9 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:smooth val="1"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Exp_data!$A$4:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:yVal>
             <c:numRef>
               <c:f>Exp_data!$B$4:$B$10</c:f>
@@ -376,11 +385,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="30053002"/>
-        <c:axId val="91101406"/>
+        <c:axId val="27310711"/>
+        <c:axId val="55018589"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30053002"/>
+        <c:axId val="27310711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,11 +405,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91101406"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="55018589"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91101406"/>
+        <c:axId val="55018589"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,8 +434,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30053002"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="27310711"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -464,16 +473,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1199880</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>31320</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>477360</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:colOff>710280</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -481,8 +490,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4826160" y="2530080"/>
-        <a:ext cx="5762160" cy="3230640"/>
+        <a:off x="7838640" y="4451760"/>
+        <a:ext cx="4326120" cy="3230280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -502,7 +511,7 @@
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K63" activeCellId="0" sqref="K63"/>
     </sheetView>
   </sheetViews>
@@ -1668,17 +1677,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3826530612245"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.2091836734694"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6530612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
@@ -1700,6 +1709,9 @@
       <c r="E1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1780,7 +1792,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1807,21 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1843,7 @@
   </sheetPr>
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1828,61 +1854,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated version of thrust_calcs and tiltangle excels. Added some pictures
</commit_message>
<xml_diff>
--- a/Thrust_Against_Mass_Calculations.xlsx
+++ b/Thrust_Against_Mass_Calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="323" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="323" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>M</t>
   </si>
@@ -64,6 +64,24 @@
     <t>Max angle (flat aluminium plate)</t>
   </si>
   <si>
+    <t>6 min 10 seconds (370 seconds). 2Nd trial: 6 min 20 secs. 55% thrust for hovering at ground level</t>
+  </si>
+  <si>
+    <t>5 min 59 seconds (353 seconds). Second trial: 6 min 19 seconds (Same thrust needed). 55% thrust for hovering above ground level</t>
+  </si>
+  <si>
+    <t>5 min 58 seconds. 55.25% thrust</t>
+  </si>
+  <si>
+    <t>5 min 58 seconds. 55.75% thrust</t>
+  </si>
+  <si>
+    <t>5 min 52 seconds (57.25% thrust)</t>
+  </si>
+  <si>
+    <t>5 min 45 seconds (57.5% thrust)</t>
+  </si>
+  <si>
     <t>very difficult to keep stable. Leave this as a question: why was it so difficult to tune this one?</t>
   </si>
   <si>
@@ -76,7 +94,7 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>6 min 45 seconds (285 seconds)</t>
+    <t>6 min 45 seconds (405 seconds). 2Nd trial 6 min 50 seconds. Thrust reqd for hovering above ground level: 50%</t>
   </si>
   <si>
     <t>Pod length (cm)</t>
@@ -351,7 +369,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:yVal>
@@ -385,11 +403,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="27310711"/>
-        <c:axId val="55018589"/>
+        <c:axId val="43893917"/>
+        <c:axId val="2759743"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27310711"/>
+        <c:axId val="43893917"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -405,11 +423,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55018589"/>
+        <c:crossAx val="2759743"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55018589"/>
+        <c:axId val="2759743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,7 +452,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27310711"/>
+        <c:crossAx val="43893917"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -473,16 +491,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>31320</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>676800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>710280</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142920</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -490,8 +508,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7838640" y="4451760"/>
-        <a:ext cx="4326120" cy="3230280"/>
+        <a:off x="5646600" y="3956040"/>
+        <a:ext cx="4325400" cy="3229560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -511,7 +529,7 @@
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K63" activeCellId="0" sqref="K63"/>
     </sheetView>
   </sheetViews>
@@ -1679,8 +1697,8 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1720,6 +1738,9 @@
       <c r="B2" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1733,6 +1754,9 @@
       <c r="B4" s="0" t="n">
         <v>63</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1749,6 +1773,9 @@
       <c r="B6" s="0" t="n">
         <v>59</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1757,6 +1784,9 @@
       <c r="B7" s="0" t="n">
         <v>52</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1765,6 +1795,9 @@
       <c r="B8" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1773,6 +1806,9 @@
       <c r="B9" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1792,7 +1828,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,21 +1843,21 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1843,8 +1879,8 @@
   </sheetPr>
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1854,61 +1890,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,16 +2038,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>2500</v>
+        <v>2300</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>0.01</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
results section on perch and hover times almost finished
</commit_message>
<xml_diff>
--- a/Thrust_Against_Mass_Calculations.xlsx
+++ b/Thrust_Against_Mass_Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="219" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="258" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6232,8 +6232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V61" sqref="V61"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6241,7 +6241,7 @@
     <col min="1" max="1" width="11.5703125"/>
     <col min="2" max="2" width="29.5703125"/>
     <col min="3" max="3" width="29.42578125"/>
-    <col min="4" max="4" width="128.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
     <col min="5" max="5" width="28.7109375"/>
     <col min="6" max="1025" width="11.5703125"/>
   </cols>
@@ -6603,7 +6603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>